<commit_message>
optimizing flexibility, day-per-day LNS, validating solutions
</commit_message>
<xml_diff>
--- a/data/matrices/distance_matrix.xlsx
+++ b/data/matrices/distance_matrix.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pierre\routage-du-coeur\data\matrices\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A2A796-7E12-4444-B407-650CDF262329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>AUTERIVE</t>
   </si>
@@ -123,13 +142,18 @@
   <si>
     <t>TOULOUSE SEMINAIRE</t>
   </si>
+  <si>
+    <t>INTER LA VACHE</t>
+  </si>
+  <si>
+    <t>METRO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +174,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -189,48 +227,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -241,34 +371,34 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="ffffff" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -282,71 +412,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -374,7 +504,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -397,11 +527,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -410,13 +540,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -426,7 +556,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -435,7 +565,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -444,7 +574,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -452,10 +582,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -520,60 +650,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AL38"/>
+  <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="AE16" workbookViewId="0">
+      <selection activeCell="AM34" sqref="AM34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="8" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="9" width="27.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="26.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="23" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="37" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2">
+      <c r="B1" s="2" t="e">
         <f>TRANSPOSE(A2:A37)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -677,12 +777,17 @@
       <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="3"/>
+      <c r="AL1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
@@ -794,9 +899,14 @@
       <c r="AK2" s="5">
         <v>16616</v>
       </c>
-      <c r="AL2" s="3"/>
+      <c r="AL2" s="17">
+        <v>1282</v>
+      </c>
+      <c r="AM2" s="15">
+        <v>3851</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -908,9 +1018,14 @@
       <c r="AK3" s="5">
         <v>37684</v>
       </c>
-      <c r="AL3" s="3"/>
+      <c r="AL3" s="17">
+        <v>39337</v>
+      </c>
+      <c r="AM3" s="15">
+        <v>40316</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1022,9 +1137,14 @@
       <c r="AK4" s="5">
         <v>133151</v>
       </c>
-      <c r="AL4" s="3"/>
+      <c r="AL4" s="17">
+        <v>145996</v>
+      </c>
+      <c r="AM4" s="15">
+        <v>146975</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1136,9 +1256,14 @@
       <c r="AK5" s="5">
         <v>43304</v>
       </c>
-      <c r="AL5" s="3"/>
+      <c r="AL5" s="17">
+        <v>31535</v>
+      </c>
+      <c r="AM5" s="15">
+        <v>33148</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1250,9 +1375,14 @@
       <c r="AK6" s="5">
         <v>14116</v>
       </c>
-      <c r="AL6" s="3"/>
+      <c r="AL6" s="17">
+        <v>7896</v>
+      </c>
+      <c r="AM6" s="15">
+        <v>6563</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1364,9 +1494,14 @@
       <c r="AK7" s="5">
         <v>38989</v>
       </c>
-      <c r="AL7" s="3"/>
+      <c r="AL7" s="17">
+        <v>46632</v>
+      </c>
+      <c r="AM7" s="15">
+        <v>47611</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:39" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1478,9 +1613,14 @@
       <c r="AK8" s="5">
         <v>53515</v>
       </c>
-      <c r="AL8" s="3"/>
+      <c r="AL8" s="17">
+        <v>63692</v>
+      </c>
+      <c r="AM8" s="15">
+        <v>64671</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1592,9 +1732,14 @@
       <c r="AK9" s="5">
         <v>10256</v>
       </c>
-      <c r="AL9" s="3"/>
+      <c r="AL9" s="17">
+        <v>19982</v>
+      </c>
+      <c r="AM9" s="15">
+        <v>20961</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1706,9 +1851,14 @@
       <c r="AK10" s="5">
         <v>28183</v>
       </c>
-      <c r="AL10" s="3"/>
+      <c r="AL10" s="17">
+        <v>23352</v>
+      </c>
+      <c r="AM10" s="15">
+        <v>24965</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1820,9 +1970,14 @@
       <c r="AK11" s="5">
         <v>20598</v>
       </c>
-      <c r="AL11" s="3"/>
+      <c r="AL11" s="17">
+        <v>6335</v>
+      </c>
+      <c r="AM11" s="15">
+        <v>6334</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1934,9 +2089,14 @@
       <c r="AK12" s="5">
         <v>9418</v>
       </c>
-      <c r="AL12" s="3"/>
+      <c r="AL12" s="17">
+        <v>23166</v>
+      </c>
+      <c r="AM12" s="15">
+        <v>24125</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -2048,9 +2208,14 @@
       <c r="AK13" s="5">
         <v>36634</v>
       </c>
-      <c r="AL13" s="3"/>
+      <c r="AL13" s="17">
+        <v>28519</v>
+      </c>
+      <c r="AM13" s="15">
+        <v>27558</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2162,9 +2327,14 @@
       <c r="AK14" s="5">
         <v>6159</v>
       </c>
-      <c r="AL14" s="3"/>
+      <c r="AL14" s="17">
+        <v>19671</v>
+      </c>
+      <c r="AM14" s="15">
+        <v>20631</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -2276,9 +2446,14 @@
       <c r="AK15" s="5">
         <v>14405</v>
       </c>
-      <c r="AL15" s="3"/>
+      <c r="AL15" s="17">
+        <v>26661</v>
+      </c>
+      <c r="AM15" s="15">
+        <v>27621</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -2390,9 +2565,14 @@
       <c r="AK16" s="5">
         <v>52852</v>
       </c>
-      <c r="AL16" s="3"/>
+      <c r="AL16" s="17">
+        <v>69954</v>
+      </c>
+      <c r="AM16" s="15">
+        <v>70914</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -2504,9 +2684,14 @@
       <c r="AK17" s="5">
         <v>100084</v>
       </c>
-      <c r="AL17" s="3"/>
+      <c r="AL17" s="17">
+        <v>109529</v>
+      </c>
+      <c r="AM17" s="15">
+        <v>110508</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2618,9 +2803,14 @@
       <c r="AK18" s="5">
         <v>17773</v>
       </c>
-      <c r="AL18" s="3"/>
+      <c r="AL18" s="17">
+        <v>25629</v>
+      </c>
+      <c r="AM18" s="15">
+        <v>26608</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -2732,9 +2922,14 @@
       <c r="AK19" s="5">
         <v>6055</v>
       </c>
-      <c r="AL19" s="3"/>
+      <c r="AL19" s="17">
+        <v>18611</v>
+      </c>
+      <c r="AM19" s="15">
+        <v>19570</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
@@ -2846,9 +3041,14 @@
       <c r="AK20" s="5">
         <v>4338</v>
       </c>
-      <c r="AL20" s="3"/>
+      <c r="AL20" s="17">
+        <v>15354</v>
+      </c>
+      <c r="AM20" s="15">
+        <v>16314</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -2960,9 +3160,14 @@
       <c r="AK21" s="5">
         <v>13983</v>
       </c>
-      <c r="AL21" s="3"/>
+      <c r="AL21" s="17">
+        <v>14717</v>
+      </c>
+      <c r="AM21" s="15">
+        <v>15696</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
@@ -3074,9 +3279,14 @@
       <c r="AK22" s="5">
         <v>66250</v>
       </c>
-      <c r="AL22" s="3"/>
+      <c r="AL22" s="17">
+        <v>59546</v>
+      </c>
+      <c r="AM22" s="15">
+        <v>61159</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
@@ -3188,9 +3398,14 @@
       <c r="AK23" s="5">
         <v>27734</v>
       </c>
-      <c r="AL23" s="3"/>
+      <c r="AL23" s="17">
+        <v>44133</v>
+      </c>
+      <c r="AM23" s="15">
+        <v>45092</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -3302,9 +3517,14 @@
       <c r="AK24" s="5">
         <v>74785</v>
       </c>
-      <c r="AL24" s="3"/>
+      <c r="AL24" s="17">
+        <v>82511</v>
+      </c>
+      <c r="AM24" s="15">
+        <v>83490</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -3416,9 +3636,14 @@
       <c r="AK25" s="5">
         <v>86883</v>
       </c>
-      <c r="AL25" s="3"/>
+      <c r="AL25" s="17">
+        <v>95687</v>
+      </c>
+      <c r="AM25" s="15">
+        <v>96666</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -3530,9 +3755,14 @@
       <c r="AK26" s="5">
         <v>11362</v>
       </c>
-      <c r="AL26" s="3"/>
+      <c r="AL26" s="17">
+        <v>7032</v>
+      </c>
+      <c r="AM26" s="15">
+        <v>7992</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row r="27" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
@@ -3644,9 +3874,14 @@
       <c r="AK27" s="5">
         <v>11016</v>
       </c>
-      <c r="AL27" s="3"/>
+      <c r="AL27" s="17">
+        <v>9058</v>
+      </c>
+      <c r="AM27" s="15">
+        <v>10037</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row r="28" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
@@ -3758,9 +3993,14 @@
       <c r="AK28" s="5">
         <v>21281</v>
       </c>
-      <c r="AL28" s="3"/>
+      <c r="AL28" s="17">
+        <v>14928</v>
+      </c>
+      <c r="AM28" s="15">
+        <v>16542</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row r="29" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
@@ -3872,9 +4112,14 @@
       <c r="AK29" s="5">
         <v>4148</v>
       </c>
-      <c r="AL29" s="3"/>
+      <c r="AL29" s="17">
+        <v>13292</v>
+      </c>
+      <c r="AM29" s="15">
+        <v>14252</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row r="30" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
@@ -3986,9 +4231,14 @@
       <c r="AK30" s="5">
         <v>48602</v>
       </c>
-      <c r="AL30" s="3"/>
+      <c r="AL30" s="17">
+        <v>42016</v>
+      </c>
+      <c r="AM30" s="15">
+        <v>43629</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
@@ -4100,9 +4350,14 @@
       <c r="AK31" s="5">
         <v>20028</v>
       </c>
-      <c r="AL31" s="3"/>
+      <c r="AL31" s="17">
+        <v>7570</v>
+      </c>
+      <c r="AM31" s="15">
+        <v>9184</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row r="32" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
@@ -4214,9 +4469,14 @@
       <c r="AK32" s="5">
         <v>22010</v>
       </c>
-      <c r="AL32" s="3"/>
+      <c r="AL32" s="17">
+        <v>15390</v>
+      </c>
+      <c r="AM32" s="15">
+        <v>17004</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row r="33" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>30</v>
       </c>
@@ -4328,9 +4588,14 @@
       <c r="AK33" s="5">
         <v>25894</v>
       </c>
-      <c r="AL33" s="3"/>
+      <c r="AL33" s="17">
+        <v>18172</v>
+      </c>
+      <c r="AM33" s="15">
+        <v>19786</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row r="34" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -4442,9 +4707,14 @@
       <c r="AK34" s="5">
         <v>12710</v>
       </c>
-      <c r="AL34" s="3"/>
+      <c r="AL34" s="17">
+        <v>9882</v>
+      </c>
+      <c r="AM34" s="15">
+        <v>10842</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row r="35" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>32</v>
       </c>
@@ -4556,9 +4826,14 @@
       <c r="AK35" s="5">
         <v>25955</v>
       </c>
-      <c r="AL35" s="3"/>
+      <c r="AL35" s="17">
+        <v>10374</v>
+      </c>
+      <c r="AM35" s="15">
+        <v>11988</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row r="36" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>33</v>
       </c>
@@ -4670,10 +4945,15 @@
       <c r="AK36" s="5">
         <v>0</v>
       </c>
-      <c r="AL36" s="3"/>
+      <c r="AL36" s="17">
+        <v>15656</v>
+      </c>
+      <c r="AM36" s="15">
+        <v>16616</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:39" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="5">
@@ -4784,49 +5064,253 @@
       <c r="AK37" s="5">
         <v>0</v>
       </c>
-      <c r="AL37" s="3"/>
+      <c r="AL37" s="17">
+        <v>15656</v>
+      </c>
+      <c r="AM37" s="15">
+        <v>16616</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="7"/>
-      <c r="V38" s="7"/>
-      <c r="W38" s="7"/>
-      <c r="X38" s="7"/>
-      <c r="Y38" s="7"/>
-      <c r="Z38" s="7"/>
-      <c r="AA38" s="7"/>
-      <c r="AB38" s="7"/>
-      <c r="AC38" s="7"/>
-      <c r="AD38" s="7"/>
-      <c r="AE38" s="7"/>
-      <c r="AF38" s="7"/>
-      <c r="AG38" s="7"/>
-      <c r="AH38" s="7"/>
-      <c r="AI38" s="7"/>
-      <c r="AJ38" s="7"/>
-      <c r="AK38" s="7"/>
-      <c r="AL38" s="6"/>
+    <row r="38" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1281</v>
+      </c>
+      <c r="C38" s="5">
+        <v>39614</v>
+      </c>
+      <c r="D38" s="5">
+        <v>146432</v>
+      </c>
+      <c r="E38" s="5">
+        <v>32424</v>
+      </c>
+      <c r="F38" s="5">
+        <v>9045</v>
+      </c>
+      <c r="G38" s="5">
+        <v>47451</v>
+      </c>
+      <c r="H38" s="5">
+        <v>64391</v>
+      </c>
+      <c r="I38" s="5">
+        <v>19755</v>
+      </c>
+      <c r="J38" s="5">
+        <v>23263</v>
+      </c>
+      <c r="K38" s="5">
+        <v>6401</v>
+      </c>
+      <c r="L38" s="5">
+        <v>24601</v>
+      </c>
+      <c r="M38" s="5">
+        <v>28713</v>
+      </c>
+      <c r="N38" s="5">
+        <v>20596</v>
+      </c>
+      <c r="O38" s="5">
+        <v>25766</v>
+      </c>
+      <c r="P38" s="5">
+        <v>70024</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>109791</v>
+      </c>
+      <c r="R38" s="5">
+        <v>23856</v>
+      </c>
+      <c r="S38" s="5">
+        <v>17366</v>
+      </c>
+      <c r="T38" s="5">
+        <v>15297</v>
+      </c>
+      <c r="U38" s="5">
+        <v>15737</v>
+      </c>
+      <c r="V38" s="5">
+        <v>66017</v>
+      </c>
+      <c r="W38" s="5">
+        <v>43539</v>
+      </c>
+      <c r="X38" s="5">
+        <v>83068</v>
+      </c>
+      <c r="Y38" s="5">
+        <v>96354</v>
+      </c>
+      <c r="Z38" s="5">
+        <v>6823</v>
+      </c>
+      <c r="AA38" s="5">
+        <v>8685</v>
+      </c>
+      <c r="AB38" s="5">
+        <v>14827</v>
+      </c>
+      <c r="AC38" s="5">
+        <v>13435</v>
+      </c>
+      <c r="AD38" s="5">
+        <v>42058</v>
+      </c>
+      <c r="AE38" s="5">
+        <v>7655</v>
+      </c>
+      <c r="AF38" s="5">
+        <v>15307</v>
+      </c>
+      <c r="AG38" s="5">
+        <v>18153</v>
+      </c>
+      <c r="AH38" s="5">
+        <v>8254</v>
+      </c>
+      <c r="AI38" s="5">
+        <v>9818</v>
+      </c>
+      <c r="AJ38" s="5">
+        <v>15527</v>
+      </c>
+      <c r="AK38" s="5">
+        <v>15527</v>
+      </c>
+      <c r="AL38" s="16">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="15">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="10">
+        <v>3870</v>
+      </c>
+      <c r="C39" s="11">
+        <v>40454</v>
+      </c>
+      <c r="D39" s="11">
+        <v>147272</v>
+      </c>
+      <c r="E39" s="11">
+        <v>34014</v>
+      </c>
+      <c r="F39" s="11">
+        <v>8484</v>
+      </c>
+      <c r="G39" s="11">
+        <v>48290</v>
+      </c>
+      <c r="H39" s="11">
+        <v>65231</v>
+      </c>
+      <c r="I39" s="11">
+        <v>20594</v>
+      </c>
+      <c r="J39" s="11">
+        <v>24854</v>
+      </c>
+      <c r="K39" s="11">
+        <v>6713</v>
+      </c>
+      <c r="L39" s="11">
+        <v>26600</v>
+      </c>
+      <c r="M39" s="11">
+        <v>28192</v>
+      </c>
+      <c r="N39" s="11">
+        <v>22596</v>
+      </c>
+      <c r="O39" s="11">
+        <v>27765</v>
+      </c>
+      <c r="P39" s="11">
+        <v>72023</v>
+      </c>
+      <c r="Q39" s="11">
+        <v>110630</v>
+      </c>
+      <c r="R39" s="11">
+        <v>24695</v>
+      </c>
+      <c r="S39" s="11">
+        <v>19365</v>
+      </c>
+      <c r="T39" s="11">
+        <v>17296</v>
+      </c>
+      <c r="U39" s="11">
+        <v>16577</v>
+      </c>
+      <c r="V39" s="11">
+        <v>67608</v>
+      </c>
+      <c r="W39" s="11">
+        <v>44378</v>
+      </c>
+      <c r="X39" s="11">
+        <v>83908</v>
+      </c>
+      <c r="Y39" s="11">
+        <v>97194</v>
+      </c>
+      <c r="Z39" s="11">
+        <v>7663</v>
+      </c>
+      <c r="AA39" s="11">
+        <v>9525</v>
+      </c>
+      <c r="AB39" s="11">
+        <v>16418</v>
+      </c>
+      <c r="AC39" s="11">
+        <v>15434</v>
+      </c>
+      <c r="AD39" s="11">
+        <v>43649</v>
+      </c>
+      <c r="AE39" s="11">
+        <v>9246</v>
+      </c>
+      <c r="AF39" s="11">
+        <v>16898</v>
+      </c>
+      <c r="AG39" s="11">
+        <v>19744</v>
+      </c>
+      <c r="AH39" s="11">
+        <v>7693</v>
+      </c>
+      <c r="AI39" s="11">
+        <v>11409</v>
+      </c>
+      <c r="AJ39" s="11">
+        <v>17526</v>
+      </c>
+      <c r="AK39" s="11">
+        <v>17526</v>
+      </c>
+      <c r="AL39" s="15">
+        <v>2730</v>
+      </c>
+      <c r="AM39" s="15">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>